<commit_message>
Added variables and removed prefix
Added variables for filename and sheetname, updated text and cancel button on dialog box
</commit_message>
<xml_diff>
--- a/XLSX Text Expander/hotstrings.xlsx
+++ b/XLSX Text Expander/hotstrings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manderson\Projects\AutoHotkey Text Expander\XLSX Text Expander\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manderson\Projects\AutoHotkey-Text-Expander\XLSX Text Expander\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88711F7E-2F38-4C9A-A5C7-909706694EA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602AB82F-0A8E-4E78-A13A-26C8DBEE1B02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1752" yWindow="1044" windowWidth="17280" windowHeight="8964" xr2:uid="{CD8A27CB-0F59-42AD-864E-142E10168CA2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{CD8A27CB-0F59-42AD-864E-142E10168CA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Templates" sheetId="3" r:id="rId1"/>
@@ -52,18 +52,6 @@
     <t>My Name</t>
   </si>
   <si>
-    <t>Marc Anderson</t>
-  </si>
-  <si>
-    <t>me</t>
-  </si>
-  <si>
-    <t>Built in shortcuts</t>
-  </si>
-  <si>
-    <t>now</t>
-  </si>
-  <si>
     <t>Current Date &amp; Time</t>
   </si>
   <si>
@@ -83,16 +71,28 @@
 That’s it, the end of the list.</t>
   </si>
   <si>
-    <t>gro</t>
-  </si>
-  <si>
-    <t>blah</t>
-  </si>
-  <si>
     <t>Ramble</t>
   </si>
   <si>
     <t>blah blah blah</t>
+  </si>
+  <si>
+    <t>&lt;ate</t>
+  </si>
+  <si>
+    <t>AutoHotkey Text Expander</t>
+  </si>
+  <si>
+    <t>now</t>
+  </si>
+  <si>
+    <t>Built in shortcuts are prefixed with &lt; symbol</t>
+  </si>
+  <si>
+    <t>&lt;list</t>
+  </si>
+  <si>
+    <t>&lt;blah</t>
   </si>
 </sst>
 </file>
@@ -450,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B039D883-0115-4888-AC93-A1EB4E1B7825}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,10 +483,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -494,10 +494,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
@@ -505,13 +505,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -519,13 +519,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A9E14EB-E2E4-4500-99FC-DAC0F6997422}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,15 +549,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update hotstring files to match
</commit_message>
<xml_diff>
--- a/XLSX Text Expander/hotstrings.xlsx
+++ b/XLSX Text Expander/hotstrings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manderson\Projects\AutoHotkey-Text-Expander\XLSX Text Expander\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xMarc\projects\autohotkey-text-expander\XLSX Text Expander\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602AB82F-0A8E-4E78-A13A-26C8DBEE1B02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9092F35-70C0-4090-A3F7-36804DD9CA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{CD8A27CB-0F59-42AD-864E-142E10168CA2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{CD8A27CB-0F59-42AD-864E-142E10168CA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Templates" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Extended Text</t>
   </si>
@@ -49,16 +49,10 @@
     <t>ID</t>
   </si>
   <si>
-    <t>My Name</t>
-  </si>
-  <si>
     <t>Current Date &amp; Time</t>
   </si>
   <si>
     <t>Greeting</t>
-  </si>
-  <si>
-    <t>Hello World!</t>
   </si>
   <si>
     <t>Grocery Note</t>
@@ -71,12 +65,6 @@
 That’s it, the end of the list.</t>
   </si>
   <si>
-    <t>Ramble</t>
-  </si>
-  <si>
-    <t>blah blah blah</t>
-  </si>
-  <si>
     <t>&lt;ate</t>
   </si>
   <si>
@@ -92,7 +80,31 @@
     <t>&lt;list</t>
   </si>
   <si>
-    <t>&lt;blah</t>
+    <t>&lt;sorry</t>
+  </si>
+  <si>
+    <t>I am sorry for the inconvenience.</t>
+  </si>
+  <si>
+    <t>&lt;hi</t>
+  </si>
+  <si>
+    <t>Hello World</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>This is a hotstring without a prefix.</t>
+  </si>
+  <si>
+    <t>Test NoPrefix Hotkey</t>
+  </si>
+  <si>
+    <t>Apology</t>
+  </si>
+  <si>
+    <t>Introduction</t>
   </si>
 </sst>
 </file>
@@ -128,9 +140,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -448,30 +459,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B039D883-0115-4888-AC93-A1EB4E1B7825}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="29.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="109.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.44140625" customWidth="1"/>
+    <col min="4" max="4" width="109.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -479,54 +488,74 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -537,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A9E14EB-E2E4-4500-99FC-DAC0F6997422}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,15 +578,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ask for input when extended text contains <<input>>
</commit_message>
<xml_diff>
--- a/XLSX Text Expander/hotstrings.xlsx
+++ b/XLSX Text Expander/hotstrings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xMarc\projects\autohotkey-text-expander\XLSX Text Expander\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9092F35-70C0-4090-A3F7-36804DD9CA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B191EA-0365-462C-9122-1FD61E73898F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{CD8A27CB-0F59-42AD-864E-142E10168CA2}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Extended Text</t>
   </si>
@@ -105,6 +105,15 @@
   </si>
   <si>
     <t>Introduction</t>
+  </si>
+  <si>
+    <t>Template Replace Input</t>
+  </si>
+  <si>
+    <t>&lt;input</t>
+  </si>
+  <si>
+    <t>&lt;&lt;input&gt;&gt;This message is for &lt;&lt;template&gt;&gt;. We are trying to reach &lt;&lt;template&gt;&gt; about their cars extended warranty.</t>
   </si>
 </sst>
 </file>
@@ -554,6 +563,20 @@
         <v>18</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D9" s="1"/>
     </row>

</xml_diff>